<commit_message>
Added Null when no data
</commit_message>
<xml_diff>
--- a/www/collab_api/storage/publications/0ArDvk7BRZ_yjdHl4OUlfUEc0ZWxpRjZyaS14aEFBLVE.xlsx
+++ b/www/collab_api/storage/publications/0ArDvk7BRZ_yjdHl4OUlfUEc0ZWxpRjZyaS14aEFBLVE.xlsx
@@ -1249,8 +1249,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0.###############"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="#,##0.###############"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1346,16 +1346,16 @@
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1" applyFill="1">
       <alignment vertical="bottom" horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="0" applyFont="1" fontId="2" applyNumberFormat="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="0" fontId="0" applyNumberFormat="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="165" borderId="0" applyFont="1" fontId="2" applyNumberFormat="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3" applyFill="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="165" borderId="0" fontId="0" applyNumberFormat="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
@@ -1380,38 +1380,38 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c t="s" s="4" r="A1">
+      <c t="s" s="5" r="A1">
         <v>0</v>
       </c>
-      <c t="s" s="4" r="B1">
+      <c t="s" s="5" r="B1">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c s="3" r="A2"/>
-      <c s="3" r="B2"/>
+      <c s="4" r="A2"/>
+      <c s="4" r="B2"/>
     </row>
     <row r="3">
-      <c t="s" s="4" r="A3">
+      <c t="s" s="5" r="A3">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="B3">
+      <c t="s" s="3" r="B3">
         <v>3</v>
       </c>
     </row>
     <row r="4">
-      <c t="s" s="4" r="A4">
+      <c t="s" s="5" r="A4">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="B4">
+      <c t="s" s="3" r="B4">
         <v>5</v>
       </c>
     </row>
     <row r="5">
-      <c t="s" s="4" r="A5">
+      <c t="s" s="5" r="A5">
         <v>6</v>
       </c>
-      <c s="2" r="B5"/>
+      <c s="3" r="B5"/>
     </row>
   </sheetData>
   <legacyDrawing r:id="rId2"/>
@@ -7914,7 +7914,7 @@
       <c t="s" r="A200">
         <v>383</v>
       </c>
-      <c s="5" r="B200">
+      <c s="2" r="B200">
         <v>17807</v>
       </c>
       <c t="s" r="C200">

</xml_diff>